<commit_message>
Ajustes solicitados por la jefe de Área
Eliminé puntos de la descripción de los recursos e incluí la descripción
general del tema.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/EsqueletoGuion_LE_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/EsqueletoGuion_LE_09_01_CO.xlsx
@@ -242,7 +242,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1543,7 +1543,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1557,13 +1557,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1630,7 +1630,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
@@ -1642,7 +1642,7 @@
     <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1676,7 +1676,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1684,7 +1684,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -1692,7 +1692,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1700,16 +1700,16 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="G12" s="7"/>
     </row>
   </sheetData>
@@ -1731,13 +1731,13 @@
       <selection activeCell="A2" sqref="A2:A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="66.140625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>33</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>34</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1">
       <c r="A4" s="13" t="s">
         <v>35</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1">
       <c r="A5" s="15" t="s">
         <v>36</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="13" t="s">
         <v>37</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="15" t="s">
         <v>38</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>39</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="15" t="s">
         <v>40</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="13" t="s">
         <v>41</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="15" t="s">
         <v>42</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="13" t="s">
         <v>43</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="15" t="s">
         <v>44</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="13" t="s">
         <v>45</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="15" t="s">
         <v>46</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="13" t="s">
         <v>47</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="15" t="s">
         <v>48</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="13" t="s">
         <v>49</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="15" t="s">
         <v>21</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="13" t="s">
         <v>22</v>
       </c>
@@ -1957,62 +1957,62 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2042,14 +2042,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="92.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="13">
         <v>11</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="13">
         <v>13</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="13">
         <v>15</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="13">
         <v>17</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="13">
         <v>19</v>
       </c>
@@ -2269,82 +2269,82 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="17"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36"/>
@@ -2372,7 +2372,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="58.85546875" customWidth="1"/>
     <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
@@ -2385,7 +2385,7 @@
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="23" t="s">
         <v>29</v>
       </c>
@@ -2431,7 +2431,7 @@
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30">
       <c r="A3" s="23" t="s">
         <v>29</v>
       </c>
@@ -2448,7 +2448,7 @@
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="23" t="s">
         <v>29</v>
       </c>
@@ -2467,7 +2467,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30">
       <c r="A5" s="23" t="s">
         <v>29</v>
       </c>
@@ -2486,7 +2486,7 @@
       <c r="H5" s="15"/>
       <c r="I5" s="24"/>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="30">
       <c r="A6" s="23" t="s">
         <v>29</v>
       </c>
@@ -2505,7 +2505,7 @@
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30">
       <c r="A7" s="23" t="s">
         <v>29</v>
       </c>
@@ -2524,7 +2524,7 @@
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30">
       <c r="A8" s="23" t="s">
         <v>29</v>
       </c>
@@ -2543,7 +2543,7 @@
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="23" t="s">
         <v>29</v>
       </c>
@@ -2562,7 +2562,7 @@
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30">
       <c r="A10" s="23" t="s">
         <v>29</v>
       </c>
@@ -2581,7 +2581,7 @@
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30">
       <c r="A11" s="23" t="s">
         <v>29</v>
       </c>
@@ -2602,7 +2602,7 @@
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30">
       <c r="A12" s="23" t="s">
         <v>29</v>
       </c>
@@ -2623,7 +2623,7 @@
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30">
       <c r="A13" s="23" t="s">
         <v>29</v>
       </c>
@@ -2644,7 +2644,7 @@
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30">
       <c r="A14" s="23" t="s">
         <v>29</v>
       </c>
@@ -2665,7 +2665,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30">
       <c r="A15" s="23" t="s">
         <v>29</v>
       </c>
@@ -2686,7 +2686,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30">
       <c r="A16" s="23" t="s">
         <v>29</v>
       </c>
@@ -2707,7 +2707,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="30">
       <c r="A17" s="23" t="s">
         <v>29</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="30">
       <c r="A18" s="23" t="s">
         <v>29</v>
       </c>
@@ -2751,7 +2751,7 @@
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="30">
       <c r="A19" s="23" t="s">
         <v>29</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30">
       <c r="A20" s="18" t="s">
         <v>29</v>
       </c>
@@ -2791,7 +2791,7 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="30">
       <c r="A21" s="18" t="s">
         <v>29</v>
       </c>
@@ -2808,7 +2808,7 @@
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="30">
       <c r="A22" s="18" t="s">
         <v>29</v>
       </c>
@@ -2825,7 +2825,7 @@
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="30">
       <c r="A23" s="18" t="s">
         <v>29</v>
       </c>
@@ -2844,7 +2844,7 @@
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="30">
       <c r="A24" s="18" t="s">
         <v>29</v>
       </c>
@@ -2863,7 +2863,7 @@
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="30">
       <c r="A25" s="18" t="s">
         <v>29</v>
       </c>
@@ -2882,7 +2882,7 @@
       <c r="H25" s="18"/>
       <c r="I25" s="18"/>
     </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="30">
       <c r="A26" s="18" t="s">
         <v>29</v>
       </c>
@@ -2901,7 +2901,7 @@
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="30">
       <c r="A27" s="18" t="s">
         <v>29</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30">
       <c r="A28" s="18" t="s">
         <v>29</v>
       </c>
@@ -2939,7 +2939,7 @@
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="30">
       <c r="A29" s="18" t="s">
         <v>29</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="30">
       <c r="A30" s="18" t="s">
         <v>29</v>
       </c>
@@ -2981,7 +2981,7 @@
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30">
       <c r="A31" s="18" t="s">
         <v>29</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="30">
       <c r="A32" s="18" t="s">
         <v>29</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="30">
       <c r="A33" s="23" t="s">
         <v>29</v>
       </c>
@@ -3044,7 +3044,7 @@
       <c r="H33" s="23"/>
       <c r="I33" s="23"/>
     </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30">
       <c r="A34" s="23" t="s">
         <v>29</v>
       </c>
@@ -3061,7 +3061,7 @@
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
     </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30">
       <c r="A35" s="23" t="s">
         <v>29</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="H35" s="23"/>
       <c r="I35" s="23"/>
     </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="30">
       <c r="A36" s="23" t="s">
         <v>29</v>
       </c>
@@ -3097,7 +3097,7 @@
       <c r="H36" s="29"/>
       <c r="I36" s="23"/>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30">
       <c r="A37" s="23" t="s">
         <v>29</v>
       </c>
@@ -3116,7 +3116,7 @@
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
     </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="30">
       <c r="A38" s="23" t="s">
         <v>29</v>
       </c>
@@ -3135,7 +3135,7 @@
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
     </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30">
       <c r="A39" s="23" t="s">
         <v>29</v>
       </c>
@@ -3154,7 +3154,7 @@
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="30">
       <c r="A40" s="23" t="s">
         <v>29</v>
       </c>
@@ -3173,7 +3173,7 @@
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
     </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="30">
       <c r="A41" s="23" t="s">
         <v>29</v>
       </c>
@@ -3192,7 +3192,7 @@
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
     </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="30">
       <c r="A42" s="23" t="s">
         <v>29</v>
       </c>
@@ -3211,7 +3211,7 @@
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
     </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30">
       <c r="A43" s="23" t="s">
         <v>29</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="30">
       <c r="A44" s="23" t="s">
         <v>29</v>
       </c>
@@ -3253,7 +3253,7 @@
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
     </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="30">
       <c r="A45" s="23" t="s">
         <v>29</v>
       </c>
@@ -3274,7 +3274,7 @@
       </c>
       <c r="I45" s="15"/>
     </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="30">
       <c r="A46" s="23" t="s">
         <v>29</v>
       </c>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="I46" s="15"/>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30">
       <c r="A47" s="18" t="s">
         <v>29</v>
       </c>
@@ -3312,7 +3312,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="30">
       <c r="A48" s="18" t="s">
         <v>29</v>
       </c>
@@ -3331,7 +3331,7 @@
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30">
       <c r="A49" s="18" t="s">
         <v>29</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="30">
       <c r="A50" s="18" t="s">
         <v>29</v>
       </c>
@@ -3373,7 +3373,7 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="30">
       <c r="A51" s="18" t="s">
         <v>29</v>
       </c>
@@ -3392,7 +3392,7 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="30">
       <c r="A52" s="18" t="s">
         <v>29</v>
       </c>
@@ -3411,7 +3411,7 @@
       <c r="H52" s="13"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="30">
       <c r="A53" s="18" t="s">
         <v>29</v>
       </c>
@@ -3430,7 +3430,7 @@
       <c r="H53" s="13"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="30">
       <c r="A54" s="18" t="s">
         <v>29</v>
       </c>
@@ -3449,7 +3449,7 @@
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="30">
       <c r="A55" s="18" t="s">
         <v>29</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="30">
       <c r="A56" s="18" t="s">
         <v>29</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" s="23" t="s">
         <v>29</v>
       </c>
@@ -3512,7 +3512,7 @@
       <c r="H57" s="31"/>
       <c r="I57" s="31"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" s="23" t="s">
         <v>29</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="23" t="s">
         <v>29</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" s="23" t="s">
         <v>29</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" s="23" t="s">
         <v>29</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62" s="23" t="s">
         <v>29</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="A63" s="23" t="s">
         <v>29</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" s="18" t="s">
         <v>29</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:64">
       <c r="A65" s="18" t="s">
         <v>29</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:64">
       <c r="A66" s="33"/>
       <c r="B66" s="34"/>
       <c r="C66" s="5"/>
@@ -3741,7 +3741,7 @@
       <c r="BK66" s="17"/>
       <c r="BL66" s="17"/>
     </row>
-    <row r="67" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:64">
       <c r="A67" s="33"/>
       <c r="B67" s="34"/>
       <c r="C67" s="5"/>
@@ -3806,7 +3806,7 @@
       <c r="BK67" s="17"/>
       <c r="BL67" s="17"/>
     </row>
-    <row r="68" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:64">
       <c r="A68" s="5"/>
       <c r="B68" s="34"/>
       <c r="C68" s="5"/>
@@ -3871,7 +3871,7 @@
       <c r="BK68" s="17"/>
       <c r="BL68" s="17"/>
     </row>
-    <row r="69" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:64">
       <c r="A69" s="5"/>
       <c r="B69" s="34"/>
       <c r="C69" s="5"/>
@@ -3936,7 +3936,7 @@
       <c r="BK69" s="17"/>
       <c r="BL69" s="17"/>
     </row>
-    <row r="70" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:64">
       <c r="A70" s="33"/>
       <c r="B70" s="35"/>
       <c r="C70" s="33"/>
@@ -4002,7 +4002,7 @@
       <c r="BK70" s="17"/>
       <c r="BL70" s="17"/>
     </row>
-    <row r="71" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:64">
       <c r="A71" s="33"/>
       <c r="B71" s="35"/>
       <c r="C71" s="33"/>
@@ -4068,7 +4068,7 @@
       <c r="BK71" s="17"/>
       <c r="BL71" s="17"/>
     </row>
-    <row r="72" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:64">
       <c r="A72" s="33"/>
       <c r="B72" s="35"/>
       <c r="C72" s="33"/>
@@ -4134,7 +4134,7 @@
       <c r="BK72" s="17"/>
       <c r="BL72" s="17"/>
     </row>
-    <row r="73" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:64">
       <c r="A73" s="33"/>
       <c r="B73" s="35"/>
       <c r="C73" s="33"/>
@@ -4200,7 +4200,7 @@
       <c r="BK73" s="17"/>
       <c r="BL73" s="17"/>
     </row>
-    <row r="74" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:64">
       <c r="A74" s="33"/>
       <c r="B74" s="35"/>
       <c r="C74" s="33"/>
@@ -4266,7 +4266,7 @@
       <c r="BK74" s="17"/>
       <c r="BL74" s="17"/>
     </row>
-    <row r="75" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:64">
       <c r="A75" s="33"/>
       <c r="B75" s="35"/>
       <c r="C75" s="33"/>
@@ -4332,7 +4332,7 @@
       <c r="BK75" s="17"/>
       <c r="BL75" s="17"/>
     </row>
-    <row r="76" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:64">
       <c r="A76" s="33"/>
       <c r="B76" s="35"/>
       <c r="C76" s="33"/>
@@ -4398,7 +4398,7 @@
       <c r="BK76" s="17"/>
       <c r="BL76" s="17"/>
     </row>
-    <row r="77" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:64">
       <c r="A77" s="33"/>
       <c r="B77" s="35"/>
       <c r="C77" s="33"/>
@@ -4464,7 +4464,7 @@
       <c r="BK77" s="17"/>
       <c r="BL77" s="17"/>
     </row>
-    <row r="78" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:64">
       <c r="A78" s="33"/>
       <c r="B78" s="35"/>
       <c r="C78" s="33"/>
@@ -4530,7 +4530,7 @@
       <c r="BK78" s="17"/>
       <c r="BL78" s="17"/>
     </row>
-    <row r="79" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:64">
       <c r="A79" s="33"/>
       <c r="B79" s="35"/>
       <c r="C79" s="33"/>
@@ -4596,7 +4596,7 @@
       <c r="BK79" s="17"/>
       <c r="BL79" s="17"/>
     </row>
-    <row r="80" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:64">
       <c r="A80" s="33"/>
       <c r="B80" s="35"/>
       <c r="C80" s="33"/>
@@ -4662,7 +4662,7 @@
       <c r="BK80" s="17"/>
       <c r="BL80" s="17"/>
     </row>
-    <row r="81" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:64">
       <c r="A81" s="33"/>
       <c r="B81" s="35"/>
       <c r="C81" s="33"/>
@@ -4728,7 +4728,7 @@
       <c r="BK81" s="17"/>
       <c r="BL81" s="17"/>
     </row>
-    <row r="82" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:64">
       <c r="A82" s="33"/>
       <c r="B82" s="35"/>
       <c r="C82" s="33"/>
@@ -4794,7 +4794,7 @@
       <c r="BK82" s="17"/>
       <c r="BL82" s="17"/>
     </row>
-    <row r="83" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:64">
       <c r="A83" s="33"/>
       <c r="B83" s="35"/>
       <c r="C83" s="33"/>
@@ -4860,7 +4860,7 @@
       <c r="BK83" s="17"/>
       <c r="BL83" s="17"/>
     </row>
-    <row r="84" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:64">
       <c r="A84" s="33"/>
       <c r="B84" s="35"/>
       <c r="C84" s="33"/>
@@ -4926,7 +4926,7 @@
       <c r="BK84" s="17"/>
       <c r="BL84" s="17"/>
     </row>
-    <row r="85" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:64">
       <c r="A85" s="33"/>
       <c r="B85" s="35"/>
       <c r="C85" s="33"/>
@@ -4992,7 +4992,7 @@
       <c r="BK85" s="17"/>
       <c r="BL85" s="17"/>
     </row>
-    <row r="86" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:64">
       <c r="A86" s="33"/>
       <c r="B86" s="35"/>
       <c r="C86" s="33"/>
@@ -5058,7 +5058,7 @@
       <c r="BK86" s="17"/>
       <c r="BL86" s="17"/>
     </row>
-    <row r="87" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:64">
       <c r="A87" s="33"/>
       <c r="B87" s="35"/>
       <c r="C87" s="33"/>
@@ -5124,7 +5124,7 @@
       <c r="BK87" s="17"/>
       <c r="BL87" s="17"/>
     </row>
-    <row r="88" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:64">
       <c r="A88" s="33"/>
       <c r="B88" s="35"/>
       <c r="C88" s="33"/>
@@ -5190,7 +5190,7 @@
       <c r="BK88" s="17"/>
       <c r="BL88" s="17"/>
     </row>
-    <row r="89" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:64">
       <c r="A89" s="33"/>
       <c r="B89" s="35"/>
       <c r="C89" s="33"/>
@@ -5256,7 +5256,7 @@
       <c r="BK89" s="17"/>
       <c r="BL89" s="17"/>
     </row>
-    <row r="90" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:64">
       <c r="A90" s="33"/>
       <c r="B90" s="35"/>
       <c r="C90" s="33"/>
@@ -5322,7 +5322,7 @@
       <c r="BK90" s="17"/>
       <c r="BL90" s="17"/>
     </row>
-    <row r="91" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:64">
       <c r="A91" s="33"/>
       <c r="B91" s="35"/>
       <c r="C91" s="33"/>
@@ -5388,7 +5388,7 @@
       <c r="BK91" s="17"/>
       <c r="BL91" s="17"/>
     </row>
-    <row r="92" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:64">
       <c r="A92" s="33"/>
       <c r="B92" s="35"/>
       <c r="C92" s="33"/>
@@ -5454,7 +5454,7 @@
       <c r="BK92" s="17"/>
       <c r="BL92" s="17"/>
     </row>
-    <row r="93" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:64">
       <c r="A93" s="33"/>
       <c r="B93" s="35"/>
       <c r="C93" s="33"/>
@@ -5520,7 +5520,7 @@
       <c r="BK93" s="17"/>
       <c r="BL93" s="17"/>
     </row>
-    <row r="94" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:64">
       <c r="A94" s="33"/>
       <c r="B94" s="35"/>
       <c r="C94" s="33"/>
@@ -5586,7 +5586,7 @@
       <c r="BK94" s="17"/>
       <c r="BL94" s="17"/>
     </row>
-    <row r="95" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:64">
       <c r="A95" s="33"/>
       <c r="B95" s="35"/>
       <c r="C95" s="33"/>
@@ -5652,7 +5652,7 @@
       <c r="BK95" s="17"/>
       <c r="BL95" s="17"/>
     </row>
-    <row r="96" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:64">
       <c r="A96" s="33"/>
       <c r="B96" s="35"/>
       <c r="C96" s="33"/>
@@ -5718,7 +5718,7 @@
       <c r="BK96" s="17"/>
       <c r="BL96" s="17"/>
     </row>
-    <row r="97" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:64">
       <c r="A97" s="33"/>
       <c r="B97" s="35"/>
       <c r="C97" s="33"/>
@@ -5784,7 +5784,7 @@
       <c r="BK97" s="17"/>
       <c r="BL97" s="17"/>
     </row>
-    <row r="98" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:64">
       <c r="A98" s="33"/>
       <c r="B98" s="35"/>
       <c r="C98" s="33"/>
@@ -5850,7 +5850,7 @@
       <c r="BK98" s="17"/>
       <c r="BL98" s="17"/>
     </row>
-    <row r="99" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:64">
       <c r="A99" s="33"/>
       <c r="B99" s="35"/>
       <c r="C99" s="33"/>
@@ -5916,7 +5916,7 @@
       <c r="BK99" s="17"/>
       <c r="BL99" s="17"/>
     </row>
-    <row r="100" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:64">
       <c r="A100" s="33"/>
       <c r="B100" s="35"/>
       <c r="C100" s="33"/>
@@ -5982,7 +5982,7 @@
       <c r="BK100" s="17"/>
       <c r="BL100" s="17"/>
     </row>
-    <row r="101" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:64">
       <c r="A101" s="33"/>
       <c r="B101" s="35"/>
       <c r="C101" s="33"/>
@@ -6048,7 +6048,7 @@
       <c r="BK101" s="17"/>
       <c r="BL101" s="17"/>
     </row>
-    <row r="102" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:64">
       <c r="A102" s="33"/>
       <c r="B102" s="35"/>
       <c r="C102" s="33"/>
@@ -6114,7 +6114,7 @@
       <c r="BK102" s="17"/>
       <c r="BL102" s="17"/>
     </row>
-    <row r="103" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:64">
       <c r="A103" s="33"/>
       <c r="B103" s="35"/>
       <c r="C103" s="33"/>
@@ -6180,7 +6180,7 @@
       <c r="BK103" s="17"/>
       <c r="BL103" s="17"/>
     </row>
-    <row r="104" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:64">
       <c r="A104" s="33"/>
       <c r="B104" s="35"/>
       <c r="C104" s="33"/>
@@ -6246,7 +6246,7 @@
       <c r="BK104" s="17"/>
       <c r="BL104" s="17"/>
     </row>
-    <row r="105" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:64">
       <c r="A105" s="33"/>
       <c r="B105" s="35"/>
       <c r="C105" s="33"/>
@@ -6312,7 +6312,7 @@
       <c r="BK105" s="17"/>
       <c r="BL105" s="17"/>
     </row>
-    <row r="106" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:64">
       <c r="A106" s="33"/>
       <c r="B106" s="35"/>
       <c r="C106" s="33"/>
@@ -6378,7 +6378,7 @@
       <c r="BK106" s="17"/>
       <c r="BL106" s="17"/>
     </row>
-    <row r="107" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:64">
       <c r="A107" s="33"/>
       <c r="B107" s="35"/>
       <c r="C107" s="33"/>
@@ -6444,7 +6444,7 @@
       <c r="BK107" s="17"/>
       <c r="BL107" s="17"/>
     </row>
-    <row r="108" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:64">
       <c r="A108" s="33"/>
       <c r="B108" s="35"/>
       <c r="C108" s="33"/>
@@ -6510,7 +6510,7 @@
       <c r="BK108" s="17"/>
       <c r="BL108" s="17"/>
     </row>
-    <row r="109" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:64">
       <c r="A109" s="33"/>
       <c r="B109" s="35"/>
       <c r="C109" s="33"/>
@@ -6576,7 +6576,7 @@
       <c r="BK109" s="17"/>
       <c r="BL109" s="17"/>
     </row>
-    <row r="110" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:64">
       <c r="A110" s="33"/>
       <c r="B110" s="35"/>
       <c r="C110" s="33"/>
@@ -6642,7 +6642,7 @@
       <c r="BK110" s="17"/>
       <c r="BL110" s="17"/>
     </row>
-    <row r="111" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:64">
       <c r="A111" s="14"/>
       <c r="B111" s="36"/>
       <c r="C111" s="14"/>
@@ -6708,7 +6708,7 @@
       <c r="BK111" s="17"/>
       <c r="BL111" s="17"/>
     </row>
-    <row r="112" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:64">
       <c r="A112" s="14"/>
       <c r="B112" s="36"/>
       <c r="C112" s="14"/>
@@ -6774,7 +6774,7 @@
       <c r="BK112" s="17"/>
       <c r="BL112" s="17"/>
     </row>
-    <row r="113" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:64">
       <c r="A113" s="5"/>
       <c r="B113" s="36"/>
       <c r="C113" s="14"/>
@@ -6839,7 +6839,7 @@
       <c r="BK113" s="17"/>
       <c r="BL113" s="17"/>
     </row>
-    <row r="114" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:64">
       <c r="A114" s="5"/>
       <c r="B114" s="36"/>
       <c r="C114" s="14"/>
@@ -6904,7 +6904,7 @@
       <c r="BK114" s="17"/>
       <c r="BL114" s="17"/>
     </row>
-    <row r="115" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:64">
       <c r="A115" s="5"/>
       <c r="B115" s="36"/>
       <c r="C115" s="14"/>
@@ -6969,7 +6969,7 @@
       <c r="BK115" s="17"/>
       <c r="BL115" s="17"/>
     </row>
-    <row r="116" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:64">
       <c r="A116" s="5"/>
       <c r="B116" s="36"/>
       <c r="C116" s="14"/>
@@ -7034,7 +7034,7 @@
       <c r="BK116" s="17"/>
       <c r="BL116" s="17"/>
     </row>
-    <row r="117" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:64">
       <c r="A117" s="5"/>
       <c r="B117" s="36"/>
       <c r="C117" s="14"/>
@@ -7099,7 +7099,7 @@
       <c r="BK117" s="17"/>
       <c r="BL117" s="17"/>
     </row>
-    <row r="118" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:64">
       <c r="A118" s="5"/>
       <c r="B118" s="36"/>
       <c r="C118" s="14"/>
@@ -7164,7 +7164,7 @@
       <c r="BK118" s="17"/>
       <c r="BL118" s="17"/>
     </row>
-    <row r="119" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:64">
       <c r="A119" s="5"/>
       <c r="B119" s="36"/>
       <c r="C119" s="14"/>
@@ -7229,7 +7229,7 @@
       <c r="BK119" s="17"/>
       <c r="BL119" s="17"/>
     </row>
-    <row r="120" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:64">
       <c r="A120" s="5"/>
       <c r="B120" s="36"/>
       <c r="C120" s="14"/>
@@ -7294,7 +7294,7 @@
       <c r="BK120" s="17"/>
       <c r="BL120" s="17"/>
     </row>
-    <row r="121" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:64">
       <c r="A121" s="5"/>
       <c r="B121" s="36"/>
       <c r="C121" s="14"/>
@@ -7359,7 +7359,7 @@
       <c r="BK121" s="17"/>
       <c r="BL121" s="17"/>
     </row>
-    <row r="122" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:64">
       <c r="A122" s="5"/>
       <c r="B122" s="36"/>
       <c r="C122" s="14"/>
@@ -7424,7 +7424,7 @@
       <c r="BK122" s="17"/>
       <c r="BL122" s="17"/>
     </row>
-    <row r="123" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:64">
       <c r="A123" s="5"/>
       <c r="B123" s="36"/>
       <c r="C123" s="14"/>
@@ -7489,7 +7489,7 @@
       <c r="BK123" s="17"/>
       <c r="BL123" s="17"/>
     </row>
-    <row r="124" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:64">
       <c r="A124" s="5"/>
       <c r="B124" s="36"/>
       <c r="C124" s="14"/>
@@ -7554,7 +7554,7 @@
       <c r="BK124" s="17"/>
       <c r="BL124" s="17"/>
     </row>
-    <row r="125" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:64">
       <c r="A125" s="5"/>
       <c r="B125" s="36"/>
       <c r="C125" s="14"/>
@@ -7619,7 +7619,7 @@
       <c r="BK125" s="17"/>
       <c r="BL125" s="17"/>
     </row>
-    <row r="126" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:64">
       <c r="A126" s="5"/>
       <c r="B126" s="36"/>
       <c r="C126" s="14"/>
@@ -7684,7 +7684,7 @@
       <c r="BK126" s="17"/>
       <c r="BL126" s="17"/>
     </row>
-    <row r="127" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:64">
       <c r="A127" s="5"/>
       <c r="B127" s="36"/>
       <c r="C127" s="14"/>
@@ -7749,7 +7749,7 @@
       <c r="BK127" s="17"/>
       <c r="BL127" s="17"/>
     </row>
-    <row r="128" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:64">
       <c r="A128" s="5"/>
       <c r="B128" s="36"/>
       <c r="C128" s="14"/>
@@ -7814,7 +7814,7 @@
       <c r="BK128" s="17"/>
       <c r="BL128" s="17"/>
     </row>
-    <row r="129" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:64">
       <c r="A129" s="5"/>
       <c r="B129" s="36"/>
       <c r="C129" s="14"/>
@@ -7879,7 +7879,7 @@
       <c r="BK129" s="17"/>
       <c r="BL129" s="17"/>
     </row>
-    <row r="130" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:64">
       <c r="A130" s="5"/>
       <c r="B130" s="36"/>
       <c r="C130" s="14"/>
@@ -7944,7 +7944,7 @@
       <c r="BK130" s="17"/>
       <c r="BL130" s="17"/>
     </row>
-    <row r="131" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:64">
       <c r="A131" s="5"/>
       <c r="B131" s="36"/>
       <c r="C131" s="14"/>
@@ -8009,7 +8009,7 @@
       <c r="BK131" s="17"/>
       <c r="BL131" s="17"/>
     </row>
-    <row r="132" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:64">
       <c r="A132" s="5"/>
       <c r="B132" s="36"/>
       <c r="C132" s="14"/>
@@ -8074,7 +8074,7 @@
       <c r="BK132" s="17"/>
       <c r="BL132" s="17"/>
     </row>
-    <row r="133" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:64">
       <c r="A133" s="5"/>
       <c r="B133" s="36"/>
       <c r="C133" s="14"/>
@@ -8139,7 +8139,7 @@
       <c r="BK133" s="17"/>
       <c r="BL133" s="17"/>
     </row>
-    <row r="134" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:64">
       <c r="A134" s="5"/>
       <c r="B134" s="36"/>
       <c r="C134" s="14"/>
@@ -8204,7 +8204,7 @@
       <c r="BK134" s="17"/>
       <c r="BL134" s="17"/>
     </row>
-    <row r="135" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:64">
       <c r="A135" s="5"/>
       <c r="B135" s="36"/>
       <c r="C135" s="14"/>
@@ -8269,7 +8269,7 @@
       <c r="BK135" s="17"/>
       <c r="BL135" s="17"/>
     </row>
-    <row r="136" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:64">
       <c r="A136" s="5"/>
       <c r="B136" s="36"/>
       <c r="C136" s="14"/>
@@ -8334,7 +8334,7 @@
       <c r="BK136" s="17"/>
       <c r="BL136" s="17"/>
     </row>
-    <row r="137" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:64">
       <c r="A137" s="5"/>
       <c r="B137" s="36"/>
       <c r="C137" s="14"/>
@@ -8399,7 +8399,7 @@
       <c r="BK137" s="17"/>
       <c r="BL137" s="17"/>
     </row>
-    <row r="138" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:64">
       <c r="A138" s="5"/>
       <c r="B138" s="36"/>
       <c r="C138" s="14"/>
@@ -8464,7 +8464,7 @@
       <c r="BK138" s="17"/>
       <c r="BL138" s="17"/>
     </row>
-    <row r="139" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:64">
       <c r="A139" s="5"/>
       <c r="B139" s="36"/>
       <c r="C139" s="14"/>
@@ -8529,7 +8529,7 @@
       <c r="BK139" s="17"/>
       <c r="BL139" s="17"/>
     </row>
-    <row r="140" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:64">
       <c r="A140" s="5"/>
       <c r="B140" s="36"/>
       <c r="C140" s="14"/>
@@ -8594,7 +8594,7 @@
       <c r="BK140" s="17"/>
       <c r="BL140" s="17"/>
     </row>
-    <row r="141" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:64">
       <c r="A141" s="5"/>
       <c r="B141" s="36"/>
       <c r="C141" s="14"/>
@@ -8659,7 +8659,7 @@
       <c r="BK141" s="17"/>
       <c r="BL141" s="17"/>
     </row>
-    <row r="142" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:64">
       <c r="A142" s="5"/>
       <c r="B142" s="36"/>
       <c r="C142" s="14"/>
@@ -8724,7 +8724,7 @@
       <c r="BK142" s="17"/>
       <c r="BL142" s="17"/>
     </row>
-    <row r="143" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:64">
       <c r="A143" s="5"/>
       <c r="B143" s="36"/>
       <c r="C143" s="14"/>
@@ -8789,7 +8789,7 @@
       <c r="BK143" s="17"/>
       <c r="BL143" s="17"/>
     </row>
-    <row r="144" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:64">
       <c r="A144" s="5"/>
       <c r="B144" s="36"/>
       <c r="C144" s="14"/>
@@ -8854,7 +8854,7 @@
       <c r="BK144" s="17"/>
       <c r="BL144" s="17"/>
     </row>
-    <row r="145" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:64">
       <c r="A145" s="5"/>
       <c r="B145" s="36"/>
       <c r="C145" s="14"/>
@@ -8919,7 +8919,7 @@
       <c r="BK145" s="17"/>
       <c r="BL145" s="17"/>
     </row>
-    <row r="146" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:64">
       <c r="A146" s="5"/>
       <c r="B146" s="36"/>
       <c r="C146" s="14"/>
@@ -8984,7 +8984,7 @@
       <c r="BK146" s="17"/>
       <c r="BL146" s="17"/>
     </row>
-    <row r="147" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:64">
       <c r="A147" s="5"/>
       <c r="B147" s="36"/>
       <c r="C147" s="14"/>
@@ -9049,7 +9049,7 @@
       <c r="BK147" s="17"/>
       <c r="BL147" s="17"/>
     </row>
-    <row r="148" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:64">
       <c r="A148" s="5"/>
       <c r="B148" s="36"/>
       <c r="C148" s="14"/>
@@ -9114,7 +9114,7 @@
       <c r="BK148" s="17"/>
       <c r="BL148" s="17"/>
     </row>
-    <row r="149" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:64">
       <c r="A149" s="5"/>
       <c r="B149" s="36"/>
       <c r="C149" s="14"/>
@@ -9179,7 +9179,7 @@
       <c r="BK149" s="17"/>
       <c r="BL149" s="17"/>
     </row>
-    <row r="150" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:64">
       <c r="A150" s="5"/>
       <c r="B150" s="36"/>
       <c r="C150" s="14"/>
@@ -9244,7 +9244,7 @@
       <c r="BK150" s="17"/>
       <c r="BL150" s="17"/>
     </row>
-    <row r="151" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:64">
       <c r="A151" s="5"/>
       <c r="B151" s="36"/>
       <c r="C151" s="14"/>
@@ -9309,7 +9309,7 @@
       <c r="BK151" s="17"/>
       <c r="BL151" s="17"/>
     </row>
-    <row r="152" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:64">
       <c r="A152" s="5"/>
       <c r="B152" s="36"/>
       <c r="C152" s="14"/>
@@ -9374,7 +9374,7 @@
       <c r="BK152" s="17"/>
       <c r="BL152" s="17"/>
     </row>
-    <row r="153" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:64">
       <c r="A153" s="5"/>
       <c r="B153" s="36"/>
       <c r="C153" s="14"/>
@@ -9439,7 +9439,7 @@
       <c r="BK153" s="17"/>
       <c r="BL153" s="17"/>
     </row>
-    <row r="154" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:64">
       <c r="A154" s="5"/>
       <c r="B154" s="36"/>
       <c r="C154" s="14"/>
@@ -9504,7 +9504,7 @@
       <c r="BK154" s="17"/>
       <c r="BL154" s="17"/>
     </row>
-    <row r="155" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:64">
       <c r="A155" s="5"/>
       <c r="B155" s="14"/>
       <c r="C155" s="14"/>
@@ -9569,7 +9569,7 @@
       <c r="BK155" s="17"/>
       <c r="BL155" s="17"/>
     </row>
-    <row r="156" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:64">
       <c r="A156" s="5"/>
       <c r="B156" s="14"/>
       <c r="C156" s="14"/>
@@ -9634,7 +9634,7 @@
       <c r="BK156" s="17"/>
       <c r="BL156" s="17"/>
     </row>
-    <row r="157" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:64">
       <c r="A157" s="5"/>
       <c r="B157" s="14"/>
       <c r="C157" s="14"/>
@@ -9699,7 +9699,7 @@
       <c r="BK157" s="17"/>
       <c r="BL157" s="17"/>
     </row>
-    <row r="158" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:64">
       <c r="A158" s="5"/>
       <c r="B158" s="14"/>
       <c r="C158" s="14"/>
@@ -9764,7 +9764,7 @@
       <c r="BK158" s="17"/>
       <c r="BL158" s="17"/>
     </row>
-    <row r="159" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:64">
       <c r="A159" s="5"/>
       <c r="B159" s="14"/>
       <c r="C159" s="14"/>
@@ -9829,7 +9829,7 @@
       <c r="BK159" s="17"/>
       <c r="BL159" s="17"/>
     </row>
-    <row r="160" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:64">
       <c r="A160" s="5"/>
       <c r="B160" s="14"/>
       <c r="C160" s="14"/>
@@ -9894,7 +9894,7 @@
       <c r="BK160" s="17"/>
       <c r="BL160" s="17"/>
     </row>
-    <row r="161" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:64">
       <c r="A161" s="17"/>
       <c r="B161" s="37"/>
       <c r="C161" s="37"/>
@@ -9959,7 +9959,7 @@
       <c r="BK161" s="17"/>
       <c r="BL161" s="17"/>
     </row>
-    <row r="162" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:64">
       <c r="A162" s="17"/>
       <c r="B162" s="37"/>
       <c r="C162" s="37"/>
@@ -10024,7 +10024,7 @@
       <c r="BK162" s="17"/>
       <c r="BL162" s="17"/>
     </row>
-    <row r="163" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:64">
       <c r="A163" s="17"/>
       <c r="B163" s="37"/>
       <c r="C163" s="37"/>
@@ -10089,7 +10089,7 @@
       <c r="BK163" s="17"/>
       <c r="BL163" s="17"/>
     </row>
-    <row r="164" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:64">
       <c r="A164" s="17"/>
       <c r="B164" s="37"/>
       <c r="C164" s="37"/>
@@ -10154,7 +10154,7 @@
       <c r="BK164" s="17"/>
       <c r="BL164" s="17"/>
     </row>
-    <row r="165" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:64">
       <c r="A165" s="17"/>
       <c r="B165" s="37"/>
       <c r="C165" s="37"/>
@@ -10219,7 +10219,7 @@
       <c r="BK165" s="17"/>
       <c r="BL165" s="17"/>
     </row>
-    <row r="166" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:64">
       <c r="A166" s="17"/>
       <c r="B166" s="37"/>
       <c r="C166" s="37"/>
@@ -10284,7 +10284,7 @@
       <c r="BK166" s="17"/>
       <c r="BL166" s="17"/>
     </row>
-    <row r="167" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:64">
       <c r="A167" s="17"/>
       <c r="B167" s="37"/>
       <c r="C167" s="37"/>
@@ -10349,7 +10349,7 @@
       <c r="BK167" s="17"/>
       <c r="BL167" s="17"/>
     </row>
-    <row r="168" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:64">
       <c r="A168" s="17"/>
       <c r="B168" s="37"/>
       <c r="C168" s="37"/>
@@ -10414,7 +10414,7 @@
       <c r="BK168" s="17"/>
       <c r="BL168" s="17"/>
     </row>
-    <row r="169" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:64">
       <c r="A169" s="17"/>
       <c r="B169" s="37"/>
       <c r="C169" s="37"/>
@@ -10479,7 +10479,7 @@
       <c r="BK169" s="17"/>
       <c r="BL169" s="17"/>
     </row>
-    <row r="170" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:64">
       <c r="A170" s="17"/>
       <c r="B170" s="37"/>
       <c r="C170" s="37"/>
@@ -10544,7 +10544,7 @@
       <c r="BK170" s="17"/>
       <c r="BL170" s="17"/>
     </row>
-    <row r="171" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:64">
       <c r="A171" s="17"/>
       <c r="B171" s="37"/>
       <c r="C171" s="37"/>
@@ -10609,7 +10609,7 @@
       <c r="BK171" s="17"/>
       <c r="BL171" s="17"/>
     </row>
-    <row r="172" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:64">
       <c r="A172" s="17"/>
       <c r="B172" s="37"/>
       <c r="C172" s="37"/>
@@ -10674,7 +10674,7 @@
       <c r="BK172" s="17"/>
       <c r="BL172" s="17"/>
     </row>
-    <row r="173" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:64">
       <c r="A173" s="17"/>
       <c r="B173" s="37"/>
       <c r="C173" s="37"/>
@@ -10739,7 +10739,7 @@
       <c r="BK173" s="17"/>
       <c r="BL173" s="17"/>
     </row>
-    <row r="174" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:64">
       <c r="A174" s="17"/>
       <c r="B174" s="37"/>
       <c r="C174" s="37"/>
@@ -10804,7 +10804,7 @@
       <c r="BK174" s="17"/>
       <c r="BL174" s="17"/>
     </row>
-    <row r="175" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:64">
       <c r="A175" s="17"/>
       <c r="B175" s="37"/>
       <c r="C175" s="37"/>
@@ -10869,7 +10869,7 @@
       <c r="BK175" s="17"/>
       <c r="BL175" s="17"/>
     </row>
-    <row r="176" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:64">
       <c r="A176" s="17"/>
       <c r="B176" s="37"/>
       <c r="C176" s="37"/>
@@ -10934,7 +10934,7 @@
       <c r="BK176" s="17"/>
       <c r="BL176" s="17"/>
     </row>
-    <row r="177" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:64">
       <c r="A177" s="17"/>
       <c r="B177" s="37"/>
       <c r="C177" s="37"/>
@@ -10999,7 +10999,7 @@
       <c r="BK177" s="17"/>
       <c r="BL177" s="17"/>
     </row>
-    <row r="178" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:64">
       <c r="A178" s="17"/>
       <c r="B178" s="37"/>
       <c r="C178" s="37"/>
@@ -11064,7 +11064,7 @@
       <c r="BK178" s="17"/>
       <c r="BL178" s="17"/>
     </row>
-    <row r="179" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:64">
       <c r="A179" s="17"/>
       <c r="B179" s="37"/>
       <c r="C179" s="37"/>
@@ -11129,7 +11129,7 @@
       <c r="BK179" s="17"/>
       <c r="BL179" s="17"/>
     </row>
-    <row r="180" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:64">
       <c r="A180" s="17"/>
       <c r="B180" s="37"/>
       <c r="C180" s="37"/>
@@ -11194,7 +11194,7 @@
       <c r="BK180" s="17"/>
       <c r="BL180" s="17"/>
     </row>
-    <row r="181" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:64">
       <c r="A181" s="17"/>
       <c r="B181" s="37"/>
       <c r="C181" s="37"/>
@@ -11259,7 +11259,7 @@
       <c r="BK181" s="17"/>
       <c r="BL181" s="17"/>
     </row>
-    <row r="182" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:64">
       <c r="A182" s="17"/>
       <c r="B182" s="37"/>
       <c r="C182" s="37"/>
@@ -11324,7 +11324,7 @@
       <c r="BK182" s="17"/>
       <c r="BL182" s="17"/>
     </row>
-    <row r="183" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:64">
       <c r="A183" s="17"/>
       <c r="B183" s="37"/>
       <c r="C183" s="37"/>
@@ -11389,7 +11389,7 @@
       <c r="BK183" s="17"/>
       <c r="BL183" s="17"/>
     </row>
-    <row r="184" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:64">
       <c r="A184" s="17"/>
       <c r="B184" s="37"/>
       <c r="C184" s="37"/>
@@ -11454,7 +11454,7 @@
       <c r="BK184" s="17"/>
       <c r="BL184" s="17"/>
     </row>
-    <row r="185" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:64">
       <c r="A185" s="17"/>
       <c r="B185" s="37"/>
       <c r="C185" s="37"/>
@@ -11519,7 +11519,7 @@
       <c r="BK185" s="17"/>
       <c r="BL185" s="17"/>
     </row>
-    <row r="186" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:64">
       <c r="A186" s="17"/>
       <c r="B186" s="37"/>
       <c r="C186" s="37"/>
@@ -11584,7 +11584,7 @@
       <c r="BK186" s="17"/>
       <c r="BL186" s="17"/>
     </row>
-    <row r="187" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:64">
       <c r="A187" s="17"/>
       <c r="B187" s="37"/>
       <c r="C187" s="37"/>
@@ -11649,7 +11649,7 @@
       <c r="BK187" s="17"/>
       <c r="BL187" s="17"/>
     </row>
-    <row r="188" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:64">
       <c r="A188" s="17"/>
       <c r="B188" s="37"/>
       <c r="C188" s="37"/>
@@ -11714,7 +11714,7 @@
       <c r="BK188" s="17"/>
       <c r="BL188" s="17"/>
     </row>
-    <row r="189" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:64">
       <c r="A189" s="17"/>
       <c r="B189" s="37"/>
       <c r="C189" s="37"/>
@@ -11779,7 +11779,7 @@
       <c r="BK189" s="17"/>
       <c r="BL189" s="17"/>
     </row>
-    <row r="190" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:64">
       <c r="A190" s="17"/>
       <c r="B190" s="37"/>
       <c r="C190" s="37"/>
@@ -11844,7 +11844,7 @@
       <c r="BK190" s="17"/>
       <c r="BL190" s="17"/>
     </row>
-    <row r="191" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:64">
       <c r="A191" s="17"/>
       <c r="B191" s="37"/>
       <c r="C191" s="37"/>
@@ -11909,7 +11909,7 @@
       <c r="BK191" s="17"/>
       <c r="BL191" s="17"/>
     </row>
-    <row r="192" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:64">
       <c r="A192" s="17"/>
       <c r="B192" s="37"/>
       <c r="C192" s="37"/>
@@ -11974,7 +11974,7 @@
       <c r="BK192" s="17"/>
       <c r="BL192" s="17"/>
     </row>
-    <row r="193" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:64">
       <c r="A193" s="17"/>
       <c r="B193" s="37"/>
       <c r="C193" s="37"/>
@@ -12039,7 +12039,7 @@
       <c r="BK193" s="17"/>
       <c r="BL193" s="17"/>
     </row>
-    <row r="194" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:64">
       <c r="A194" s="17"/>
       <c r="B194" s="37"/>
       <c r="C194" s="37"/>
@@ -12104,7 +12104,7 @@
       <c r="BK194" s="17"/>
       <c r="BL194" s="17"/>
     </row>
-    <row r="195" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:64">
       <c r="A195" s="17"/>
       <c r="B195" s="37"/>
       <c r="C195" s="37"/>
@@ -12169,7 +12169,7 @@
       <c r="BK195" s="17"/>
       <c r="BL195" s="17"/>
     </row>
-    <row r="196" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:64">
       <c r="A196" s="17"/>
       <c r="B196" s="37"/>
       <c r="C196" s="37"/>
@@ -12234,7 +12234,7 @@
       <c r="BK196" s="17"/>
       <c r="BL196" s="17"/>
     </row>
-    <row r="197" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:64">
       <c r="A197" s="17"/>
       <c r="B197" s="37"/>
       <c r="C197" s="37"/>
@@ -12299,7 +12299,7 @@
       <c r="BK197" s="17"/>
       <c r="BL197" s="17"/>
     </row>
-    <row r="198" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:64">
       <c r="A198" s="17"/>
       <c r="B198" s="37"/>
       <c r="C198" s="37"/>
@@ -12364,7 +12364,7 @@
       <c r="BK198" s="17"/>
       <c r="BL198" s="17"/>
     </row>
-    <row r="199" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:64">
       <c r="A199" s="17"/>
       <c r="B199" s="37"/>
       <c r="C199" s="37"/>
@@ -12429,7 +12429,7 @@
       <c r="BK199" s="17"/>
       <c r="BL199" s="17"/>
     </row>
-    <row r="200" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:64">
       <c r="A200" s="17"/>
       <c r="B200" s="37"/>
       <c r="C200" s="37"/>
@@ -12494,7 +12494,7 @@
       <c r="BK200" s="17"/>
       <c r="BL200" s="17"/>
     </row>
-    <row r="201" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:64">
       <c r="A201" s="17"/>
       <c r="B201" s="37"/>
       <c r="C201" s="37"/>
@@ -12559,7 +12559,7 @@
       <c r="BK201" s="17"/>
       <c r="BL201" s="17"/>
     </row>
-    <row r="202" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:64">
       <c r="A202" s="17"/>
       <c r="B202" s="37"/>
       <c r="C202" s="37"/>
@@ -12624,7 +12624,7 @@
       <c r="BK202" s="17"/>
       <c r="BL202" s="17"/>
     </row>
-    <row r="203" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:64">
       <c r="A203" s="17"/>
       <c r="B203" s="37"/>
       <c r="C203" s="37"/>
@@ -12689,7 +12689,7 @@
       <c r="BK203" s="17"/>
       <c r="BL203" s="17"/>
     </row>
-    <row r="204" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:64">
       <c r="A204" s="17"/>
       <c r="B204" s="37"/>
       <c r="C204" s="37"/>
@@ -12754,7 +12754,7 @@
       <c r="BK204" s="17"/>
       <c r="BL204" s="17"/>
     </row>
-    <row r="205" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:64">
       <c r="A205" s="17"/>
       <c r="B205" s="37"/>
       <c r="C205" s="37"/>
@@ -12819,7 +12819,7 @@
       <c r="BK205" s="17"/>
       <c r="BL205" s="17"/>
     </row>
-    <row r="206" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:64">
       <c r="A206" s="17"/>
       <c r="B206" s="37"/>
       <c r="C206" s="37"/>
@@ -12884,7 +12884,7 @@
       <c r="BK206" s="17"/>
       <c r="BL206" s="17"/>
     </row>
-    <row r="207" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:64">
       <c r="A207" s="17"/>
       <c r="B207" s="37"/>
       <c r="C207" s="37"/>
@@ -12949,7 +12949,7 @@
       <c r="BK207" s="17"/>
       <c r="BL207" s="17"/>
     </row>
-    <row r="208" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:64">
       <c r="A208" s="17"/>
       <c r="B208" s="37"/>
       <c r="C208" s="37"/>
@@ -13014,7 +13014,7 @@
       <c r="BK208" s="17"/>
       <c r="BL208" s="17"/>
     </row>
-    <row r="209" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:64">
       <c r="A209" s="17"/>
       <c r="B209" s="37"/>
       <c r="C209" s="37"/>
@@ -13079,7 +13079,7 @@
       <c r="BK209" s="17"/>
       <c r="BL209" s="17"/>
     </row>
-    <row r="210" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:64">
       <c r="A210" s="17"/>
       <c r="B210" s="37"/>
       <c r="C210" s="37"/>
@@ -13144,7 +13144,7 @@
       <c r="BK210" s="17"/>
       <c r="BL210" s="17"/>
     </row>
-    <row r="211" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:64">
       <c r="A211" s="17"/>
       <c r="B211" s="37"/>
       <c r="C211" s="37"/>
@@ -13209,7 +13209,7 @@
       <c r="BK211" s="17"/>
       <c r="BL211" s="17"/>
     </row>
-    <row r="212" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:64">
       <c r="A212" s="17"/>
       <c r="B212" s="37"/>
       <c r="C212" s="37"/>
@@ -13274,7 +13274,7 @@
       <c r="BK212" s="17"/>
       <c r="BL212" s="17"/>
     </row>
-    <row r="213" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:64">
       <c r="A213" s="17"/>
       <c r="B213" s="37"/>
       <c r="C213" s="37"/>
@@ -13339,7 +13339,7 @@
       <c r="BK213" s="17"/>
       <c r="BL213" s="17"/>
     </row>
-    <row r="214" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:64">
       <c r="A214" s="17"/>
       <c r="B214" s="37"/>
       <c r="C214" s="37"/>
@@ -13404,7 +13404,7 @@
       <c r="BK214" s="17"/>
       <c r="BL214" s="17"/>
     </row>
-    <row r="215" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:64">
       <c r="A215" s="17"/>
       <c r="B215" s="37"/>
       <c r="C215" s="37"/>
@@ -13469,7 +13469,7 @@
       <c r="BK215" s="17"/>
       <c r="BL215" s="17"/>
     </row>
-    <row r="216" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:64">
       <c r="A216" s="17"/>
       <c r="B216" s="37"/>
       <c r="C216" s="37"/>
@@ -13534,7 +13534,7 @@
       <c r="BK216" s="17"/>
       <c r="BL216" s="17"/>
     </row>
-    <row r="217" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:64">
       <c r="A217" s="17"/>
       <c r="B217" s="37"/>
       <c r="C217" s="37"/>
@@ -13599,7 +13599,7 @@
       <c r="BK217" s="17"/>
       <c r="BL217" s="17"/>
     </row>
-    <row r="218" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:64">
       <c r="A218" s="17"/>
       <c r="B218" s="37"/>
       <c r="C218" s="37"/>
@@ -13664,7 +13664,7 @@
       <c r="BK218" s="17"/>
       <c r="BL218" s="17"/>
     </row>
-    <row r="219" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:64">
       <c r="A219" s="17"/>
       <c r="B219" s="37"/>
       <c r="C219" s="37"/>
@@ -13729,7 +13729,7 @@
       <c r="BK219" s="17"/>
       <c r="BL219" s="17"/>
     </row>
-    <row r="220" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:64">
       <c r="A220" s="17"/>
       <c r="B220" s="37"/>
       <c r="C220" s="37"/>
@@ -13794,7 +13794,7 @@
       <c r="BK220" s="17"/>
       <c r="BL220" s="17"/>
     </row>
-    <row r="221" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:64">
       <c r="A221" s="17"/>
       <c r="B221" s="37"/>
       <c r="C221" s="37"/>
@@ -13859,7 +13859,7 @@
       <c r="BK221" s="17"/>
       <c r="BL221" s="17"/>
     </row>
-    <row r="222" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:64">
       <c r="A222" s="17"/>
       <c r="B222" s="37"/>
       <c r="C222" s="37"/>
@@ -13924,7 +13924,7 @@
       <c r="BK222" s="17"/>
       <c r="BL222" s="17"/>
     </row>
-    <row r="223" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:64">
       <c r="A223" s="17"/>
       <c r="B223" s="37"/>
       <c r="C223" s="37"/>
@@ -13989,7 +13989,7 @@
       <c r="BK223" s="17"/>
       <c r="BL223" s="17"/>
     </row>
-    <row r="224" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:64">
       <c r="A224" s="17"/>
       <c r="B224" s="37"/>
       <c r="C224" s="37"/>
@@ -14054,7 +14054,7 @@
       <c r="BK224" s="17"/>
       <c r="BL224" s="17"/>
     </row>
-    <row r="225" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:64">
       <c r="A225" s="17"/>
       <c r="B225" s="37"/>
       <c r="C225" s="37"/>
@@ -14119,7 +14119,7 @@
       <c r="BK225" s="17"/>
       <c r="BL225" s="17"/>
     </row>
-    <row r="226" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:64">
       <c r="A226" s="17"/>
       <c r="B226" s="37"/>
       <c r="C226" s="37"/>
@@ -14184,7 +14184,7 @@
       <c r="BK226" s="17"/>
       <c r="BL226" s="17"/>
     </row>
-    <row r="227" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:64">
       <c r="A227" s="17"/>
       <c r="B227" s="37"/>
       <c r="C227" s="37"/>
@@ -14249,7 +14249,7 @@
       <c r="BK227" s="17"/>
       <c r="BL227" s="17"/>
     </row>
-    <row r="228" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:64">
       <c r="A228" s="17"/>
       <c r="B228" s="37"/>
       <c r="C228" s="37"/>
@@ -14314,7 +14314,7 @@
       <c r="BK228" s="17"/>
       <c r="BL228" s="17"/>
     </row>
-    <row r="229" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:64">
       <c r="A229" s="17"/>
       <c r="B229" s="37"/>
       <c r="C229" s="37"/>
@@ -14379,7 +14379,7 @@
       <c r="BK229" s="17"/>
       <c r="BL229" s="17"/>
     </row>
-    <row r="230" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:64">
       <c r="A230" s="17"/>
       <c r="B230" s="37"/>
       <c r="C230" s="37"/>
@@ -14444,7 +14444,7 @@
       <c r="BK230" s="17"/>
       <c r="BL230" s="17"/>
     </row>
-    <row r="231" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:64">
       <c r="A231" s="17"/>
       <c r="B231" s="37"/>
       <c r="C231" s="37"/>
@@ -14509,7 +14509,7 @@
       <c r="BK231" s="17"/>
       <c r="BL231" s="17"/>
     </row>
-    <row r="232" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:64">
       <c r="A232" s="17"/>
       <c r="B232" s="37"/>
       <c r="C232" s="37"/>
@@ -14574,7 +14574,7 @@
       <c r="BK232" s="17"/>
       <c r="BL232" s="17"/>
     </row>
-    <row r="233" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:64">
       <c r="A233" s="17"/>
       <c r="B233" s="37"/>
       <c r="C233" s="37"/>
@@ -14639,7 +14639,7 @@
       <c r="BK233" s="17"/>
       <c r="BL233" s="17"/>
     </row>
-    <row r="234" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:64">
       <c r="A234" s="17"/>
       <c r="B234" s="37"/>
       <c r="C234" s="37"/>
@@ -14704,7 +14704,7 @@
       <c r="BK234" s="17"/>
       <c r="BL234" s="17"/>
     </row>
-    <row r="235" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:64">
       <c r="A235" s="17"/>
       <c r="B235" s="37"/>
       <c r="C235" s="37"/>
@@ -14769,7 +14769,7 @@
       <c r="BK235" s="17"/>
       <c r="BL235" s="17"/>
     </row>
-    <row r="236" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:64">
       <c r="A236" s="17"/>
       <c r="B236" s="37"/>
       <c r="C236" s="37"/>
@@ -14834,7 +14834,7 @@
       <c r="BK236" s="17"/>
       <c r="BL236" s="17"/>
     </row>
-    <row r="237" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:64">
       <c r="A237" s="17"/>
       <c r="B237" s="37"/>
       <c r="C237" s="37"/>
@@ -14899,7 +14899,7 @@
       <c r="BK237" s="17"/>
       <c r="BL237" s="17"/>
     </row>
-    <row r="238" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:64">
       <c r="A238" s="17"/>
       <c r="B238" s="37"/>
       <c r="C238" s="37"/>
@@ -14964,7 +14964,7 @@
       <c r="BK238" s="17"/>
       <c r="BL238" s="17"/>
     </row>
-    <row r="239" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:64">
       <c r="A239" s="17"/>
       <c r="B239" s="37"/>
       <c r="C239" s="37"/>
@@ -15029,7 +15029,7 @@
       <c r="BK239" s="17"/>
       <c r="BL239" s="17"/>
     </row>
-    <row r="240" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:64">
       <c r="A240" s="17"/>
       <c r="B240" s="37"/>
       <c r="C240" s="37"/>
@@ -15094,7 +15094,7 @@
       <c r="BK240" s="17"/>
       <c r="BL240" s="17"/>
     </row>
-    <row r="241" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:64">
       <c r="A241" s="17"/>
       <c r="B241" s="37"/>
       <c r="C241" s="37"/>
@@ -15159,7 +15159,7 @@
       <c r="BK241" s="17"/>
       <c r="BL241" s="17"/>
     </row>
-    <row r="242" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:64">
       <c r="A242" s="17"/>
       <c r="B242" s="37"/>
       <c r="C242" s="37"/>
@@ -15224,7 +15224,7 @@
       <c r="BK242" s="17"/>
       <c r="BL242" s="17"/>
     </row>
-    <row r="243" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:64">
       <c r="A243" s="17"/>
       <c r="B243" s="37"/>
       <c r="C243" s="37"/>
@@ -15289,7 +15289,7 @@
       <c r="BK243" s="17"/>
       <c r="BL243" s="17"/>
     </row>
-    <row r="244" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:64">
       <c r="A244" s="17"/>
       <c r="B244" s="37"/>
       <c r="C244" s="37"/>
@@ -15354,7 +15354,7 @@
       <c r="BK244" s="17"/>
       <c r="BL244" s="17"/>
     </row>
-    <row r="245" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:64">
       <c r="A245" s="17"/>
       <c r="B245" s="37"/>
       <c r="C245" s="37"/>
@@ -15419,7 +15419,7 @@
       <c r="BK245" s="17"/>
       <c r="BL245" s="17"/>
     </row>
-    <row r="246" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:64">
       <c r="A246" s="17"/>
       <c r="B246" s="37"/>
       <c r="C246" s="37"/>
@@ -15484,7 +15484,7 @@
       <c r="BK246" s="17"/>
       <c r="BL246" s="17"/>
     </row>
-    <row r="247" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:64">
       <c r="A247" s="17"/>
       <c r="B247" s="37"/>
       <c r="C247" s="37"/>
@@ -15549,7 +15549,7 @@
       <c r="BK247" s="17"/>
       <c r="BL247" s="17"/>
     </row>
-    <row r="248" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:64">
       <c r="A248" s="17"/>
       <c r="B248" s="37"/>
       <c r="C248" s="37"/>
@@ -15614,7 +15614,7 @@
       <c r="BK248" s="17"/>
       <c r="BL248" s="17"/>
     </row>
-    <row r="249" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:64">
       <c r="A249" s="17"/>
       <c r="B249" s="37"/>
       <c r="C249" s="37"/>
@@ -15679,7 +15679,7 @@
       <c r="BK249" s="17"/>
       <c r="BL249" s="17"/>
     </row>
-    <row r="250" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:64">
       <c r="A250" s="17"/>
       <c r="B250" s="37"/>
       <c r="C250" s="37"/>
@@ -15744,7 +15744,7 @@
       <c r="BK250" s="17"/>
       <c r="BL250" s="17"/>
     </row>
-    <row r="251" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:64">
       <c r="A251" s="17"/>
       <c r="B251" s="37"/>
       <c r="C251" s="37"/>
@@ -15809,7 +15809,7 @@
       <c r="BK251" s="17"/>
       <c r="BL251" s="17"/>
     </row>
-    <row r="252" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:64">
       <c r="A252" s="17"/>
       <c r="B252" s="37"/>
       <c r="C252" s="37"/>
@@ -15874,7 +15874,7 @@
       <c r="BK252" s="17"/>
       <c r="BL252" s="17"/>
     </row>
-    <row r="253" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:64">
       <c r="A253" s="17"/>
       <c r="B253" s="37"/>
       <c r="C253" s="37"/>
@@ -15939,7 +15939,7 @@
       <c r="BK253" s="17"/>
       <c r="BL253" s="17"/>
     </row>
-    <row r="254" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:64">
       <c r="A254" s="17"/>
       <c r="B254" s="37"/>
       <c r="C254" s="37"/>
@@ -16004,7 +16004,7 @@
       <c r="BK254" s="17"/>
       <c r="BL254" s="17"/>
     </row>
-    <row r="255" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:64">
       <c r="A255" s="17"/>
       <c r="B255" s="37"/>
       <c r="C255" s="37"/>
@@ -16069,7 +16069,7 @@
       <c r="BK255" s="17"/>
       <c r="BL255" s="17"/>
     </row>
-    <row r="256" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:64">
       <c r="A256" s="17"/>
       <c r="B256" s="37"/>
       <c r="C256" s="37"/>
@@ -16134,7 +16134,7 @@
       <c r="BK256" s="17"/>
       <c r="BL256" s="17"/>
     </row>
-    <row r="257" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:64">
       <c r="A257" s="17"/>
       <c r="B257" s="37"/>
       <c r="C257" s="37"/>
@@ -16199,7 +16199,7 @@
       <c r="BK257" s="17"/>
       <c r="BL257" s="17"/>
     </row>
-    <row r="258" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:64">
       <c r="A258" s="17"/>
       <c r="B258" s="37"/>
       <c r="C258" s="37"/>
@@ -16264,7 +16264,7 @@
       <c r="BK258" s="17"/>
       <c r="BL258" s="17"/>
     </row>
-    <row r="259" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:64">
       <c r="A259" s="17"/>
       <c r="B259" s="37"/>
       <c r="C259" s="37"/>
@@ -16329,7 +16329,7 @@
       <c r="BK259" s="17"/>
       <c r="BL259" s="17"/>
     </row>
-    <row r="260" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:64">
       <c r="A260" s="17"/>
       <c r="B260" s="37"/>
       <c r="C260" s="37"/>
@@ -16394,7 +16394,7 @@
       <c r="BK260" s="17"/>
       <c r="BL260" s="17"/>
     </row>
-    <row r="261" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:64">
       <c r="A261" s="17"/>
       <c r="B261" s="37"/>
       <c r="C261" s="37"/>
@@ -16459,7 +16459,7 @@
       <c r="BK261" s="17"/>
       <c r="BL261" s="17"/>
     </row>
-    <row r="262" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:64">
       <c r="A262" s="17"/>
       <c r="B262" s="37"/>
       <c r="C262" s="37"/>
@@ -16524,7 +16524,7 @@
       <c r="BK262" s="17"/>
       <c r="BL262" s="17"/>
     </row>
-    <row r="263" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:64">
       <c r="A263" s="17"/>
       <c r="B263" s="37"/>
       <c r="C263" s="37"/>
@@ -16589,7 +16589,7 @@
       <c r="BK263" s="17"/>
       <c r="BL263" s="17"/>
     </row>
-    <row r="264" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:64">
       <c r="A264" s="17"/>
       <c r="B264" s="37"/>
       <c r="C264" s="37"/>
@@ -16654,7 +16654,7 @@
       <c r="BK264" s="17"/>
       <c r="BL264" s="17"/>
     </row>
-    <row r="265" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:64">
       <c r="A265" s="17"/>
       <c r="B265" s="37"/>
       <c r="C265" s="37"/>
@@ -16719,7 +16719,7 @@
       <c r="BK265" s="17"/>
       <c r="BL265" s="17"/>
     </row>
-    <row r="266" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:64">
       <c r="A266" s="17"/>
       <c r="B266" s="37"/>
       <c r="C266" s="37"/>
@@ -16784,7 +16784,7 @@
       <c r="BK266" s="17"/>
       <c r="BL266" s="17"/>
     </row>
-    <row r="267" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:64">
       <c r="A267" s="17"/>
       <c r="B267" s="37"/>
       <c r="C267" s="37"/>
@@ -16849,7 +16849,7 @@
       <c r="BK267" s="17"/>
       <c r="BL267" s="17"/>
     </row>
-    <row r="268" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:64">
       <c r="A268" s="17"/>
       <c r="B268" s="37"/>
       <c r="C268" s="37"/>
@@ -16914,7 +16914,7 @@
       <c r="BK268" s="17"/>
       <c r="BL268" s="17"/>
     </row>
-    <row r="269" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:64">
       <c r="A269" s="17"/>
       <c r="B269" s="37"/>
       <c r="C269" s="37"/>
@@ -16979,7 +16979,7 @@
       <c r="BK269" s="17"/>
       <c r="BL269" s="17"/>
     </row>
-    <row r="270" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:64">
       <c r="A270" s="17"/>
       <c r="B270" s="37"/>
       <c r="C270" s="37"/>

</xml_diff>